<commit_message>
-Finalize report percentage monthly report
</commit_message>
<xml_diff>
--- a/GRis/Content/ExcelTemplates/ServerSalariesPercentageMonthlyReportTemplate.xlsx
+++ b/GRis/Content/ExcelTemplates/ServerSalariesPercentageMonthlyReportTemplate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="11">
   <si>
     <t>NAME</t>
   </si>
@@ -394,7 +394,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -445,7 +445,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -464,72 +464,138 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>